<commit_message>
update: RO and ERD
</commit_message>
<xml_diff>
--- a/docs/RequirementOutline.xlsx
+++ b/docs/RequirementOutline.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="10187"/>
+    <workbookView windowWidth="23040" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="RO" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="101">
   <si>
     <t>Requirement Outline</t>
   </si>
@@ -298,7 +298,7 @@
     <t>+ Tìm kiếm loại bàn theo tên loại (tương đối)</t>
   </si>
   <si>
-    <t>- Mỗi loại bàn có số tiền/giờ khác nhau</t>
+    <t>- Mỗi loại bàn phải có số tiền/giờ (Số tiền trên mỗi giờ chơi)</t>
   </si>
   <si>
     <t>- Mỗi bàn phải và chỉ thuộc 1 loại bàn</t>
@@ -352,7 +352,10 @@
     <t>- Nếu số giờ chơi của hội viên &gt;= số giờ chơi của một cấp độ và không &gt;= số giờ chơi của cấp độ nào nữa thì hội viên sẽ đạt được cấp độ đó</t>
   </si>
   <si>
-    <t>- Mỗi cấp độ hội viên sẽ có một mức ưu đãi nhất định (VD: cấp độ "đồng" tương ứng giảm 5%/tổng hóa đơn, "bạc" - 10%/tổng hóa đơn,...)</t>
+    <t>- Mỗi cấp độ hội viên sẽ được giảm ?% / tổng hóa đơn (VD: cấp độ "đồng" tương ứng giảm 5%/tổng hóa đơn, "bạc" - 10%/tổng hóa đơn,...)</t>
+  </si>
+  <si>
+    <t>- Cập độ hội viên có số giờ chơi yêu cầu lớn hơn thì sẽ có % giảm giá trên tổng hóa đơn &gt; hơn</t>
   </si>
   <si>
     <t>- Quản lý hội viên</t>
@@ -1560,8 +1563,8 @@
   <sheetPr/>
   <dimension ref="A1:Z1073"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="M105" sqref="M105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4259259259259" defaultRowHeight="15" customHeight="1"/>
@@ -4645,7 +4648,9 @@
       <c r="B105" s="3"/>
       <c r="C105" s="1"/>
       <c r="D105" s="1"/>
-      <c r="E105" s="1"/>
+      <c r="E105" s="8" t="s">
+        <v>81</v>
+      </c>
       <c r="F105" s="1"/>
       <c r="G105" s="1"/>
       <c r="H105" s="1"/>
@@ -4672,7 +4677,7 @@
       <c r="A106" s="1"/>
       <c r="B106" s="3"/>
       <c r="C106" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D106" s="1"/>
       <c r="E106" s="1"/>
@@ -4703,7 +4708,7 @@
       <c r="B107" s="3"/>
       <c r="C107" s="1"/>
       <c r="D107" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E107" s="1"/>
       <c r="F107" s="1"/>
@@ -4733,7 +4738,7 @@
       <c r="B108" s="3"/>
       <c r="C108" s="1"/>
       <c r="D108" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E108" s="1"/>
       <c r="F108" s="1"/>
@@ -4763,7 +4768,7 @@
       <c r="B109" s="3"/>
       <c r="C109" s="1"/>
       <c r="D109" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E109" s="1"/>
       <c r="F109" s="1"/>
@@ -4793,7 +4798,7 @@
       <c r="B110" s="3"/>
       <c r="C110" s="1"/>
       <c r="D110" s="8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E110" s="1"/>
       <c r="F110" s="1"/>
@@ -4854,7 +4859,7 @@
       <c r="C112" s="1"/>
       <c r="D112" s="1"/>
       <c r="E112" s="8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F112" s="1"/>
       <c r="G112" s="1"/>
@@ -4910,7 +4915,7 @@
       <c r="A114" s="1"/>
       <c r="B114" s="3"/>
       <c r="C114" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D114" s="1"/>
       <c r="E114" s="1"/>
@@ -4941,7 +4946,7 @@
       <c r="B115" s="3"/>
       <c r="C115" s="1"/>
       <c r="D115" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E115" s="1"/>
       <c r="F115" s="1"/>
@@ -4971,7 +4976,7 @@
       <c r="B116" s="3"/>
       <c r="C116" s="1"/>
       <c r="D116" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E116" s="1"/>
       <c r="F116" s="1"/>
@@ -5001,7 +5006,7 @@
       <c r="B117" s="3"/>
       <c r="C117" s="1"/>
       <c r="D117" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E117" s="1"/>
       <c r="F117" s="1"/>
@@ -5031,7 +5036,7 @@
       <c r="B118" s="3"/>
       <c r="C118" s="1"/>
       <c r="D118" s="8" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E118" s="1"/>
       <c r="F118" s="1"/>
@@ -5061,7 +5066,7 @@
       <c r="B119" s="3"/>
       <c r="C119" s="1"/>
       <c r="D119" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E119" s="1"/>
       <c r="F119" s="1"/>
@@ -5091,7 +5096,7 @@
       <c r="B120" s="3"/>
       <c r="C120" s="1"/>
       <c r="D120" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E120" s="1"/>
       <c r="F120" s="1"/>
@@ -5152,7 +5157,7 @@
       <c r="C122" s="1"/>
       <c r="D122" s="1"/>
       <c r="E122" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F122" s="1"/>
       <c r="G122" s="1"/>
@@ -5208,7 +5213,7 @@
       <c r="A124" s="1"/>
       <c r="B124" s="3"/>
       <c r="C124" s="8" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D124" s="1"/>
       <c r="E124" s="1"/>
@@ -5265,7 +5270,7 @@
     <row r="126" customHeight="1" spans="1:26">
       <c r="A126" s="1"/>
       <c r="B126" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C126" s="1"/>
       <c r="D126" s="1"/>
@@ -5296,7 +5301,7 @@
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D127" s="1"/>
       <c r="E127" s="1"/>
@@ -5326,7 +5331,7 @@
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D128" s="1"/>
       <c r="E128" s="1"/>
@@ -5356,7 +5361,7 @@
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="8" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D129" s="1"/>
       <c r="E129" s="1"/>

</xml_diff>